<commit_message>
Deploy IG build 1dbb6cea7af271453a6073999d7b108afd2fd71d
</commit_message>
<xml_diff>
--- a/currentbuild/StructureDefinition-no-basis-Address.xlsx
+++ b/currentbuild/StructureDefinition-no-basis-Address.xlsx
@@ -381,7 +381,7 @@
     <t>propertyInformation</t>
   </si>
   <si>
-    <t xml:space="preserve">Extension {http://hl7.no/fhir/ig/StructureDefinition/no-basis-propertyinformation}
+    <t xml:space="preserve">Extension {http://hl7.no/fhir/StructureDefinition/no-basis-propertyinformation}
 </t>
   </si>
   <si>
@@ -593,7 +593,7 @@
     <t>municipalitycode</t>
   </si>
   <si>
-    <t xml:space="preserve">Extension {http://hl7.no/fhir/ig/StructureDefinition/no-basis-municipalitycode}
+    <t xml:space="preserve">Extension {http://hl7.no/fhir/StructureDefinition/no-basis-municipalitycode}
 </t>
   </si>
   <si>
@@ -1041,7 +1041,7 @@
     <col min="8" max="8" width="13.953125" customWidth="true" bestFit="true"/>
     <col min="9" max="9" width="11.3671875" customWidth="true" bestFit="true"/>
     <col min="10" max="10" width="20.703125" customWidth="true" bestFit="true"/>
-    <col min="11" max="11" width="64.94921875" customWidth="true" bestFit="true"/>
+    <col min="11" max="11" width="62.984375" customWidth="true" bestFit="true"/>
     <col min="12" max="12" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="13" max="13" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="14" max="14" width="100.703125" customWidth="true" bestFit="true"/>

</xml_diff>